<commit_message>
intorduced switch so that it can be used with old/new veda
</commit_message>
<xml_diff>
--- a/Syssettings.xlsx
+++ b/Syssettings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\DemoS_ADV_Stuttgart061118\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\adv demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E0AEA5-64EC-4A9A-AE1D-9E04F1B854DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E136032-DC49-4707-8F1F-D9CA4D0A5B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="195">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -781,12 +781,6 @@
   </si>
   <si>
     <t>~TFM_INS-txt</t>
-  </si>
-  <si>
-    <t>~TFM_MIG</t>
-  </si>
-  <si>
-    <t>Year2</t>
   </si>
 </sst>
 </file>
@@ -799,7 +793,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -902,8 +896,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -976,8 +977,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1158,8 +1164,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -1168,8 +1189,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1471,8 +1493,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="16" xfId="8"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="Input" xfId="8" builtinId="20"/>
     <cellStyle name="Migliaia_tab emissioni" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -4413,11 +4437,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B3:Q36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4430,12 +4452,18 @@
     <col min="13" max="13" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="str">
+        <f>IF($A$1=1,"~TFM_MIG","~TFM_UPD")</f>
+        <v>~TFM_MIG</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
@@ -4445,8 +4473,9 @@
       <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>196</v>
+      <c r="E4" s="5" t="str">
+        <f>IF($A$1=1,"year2","year")</f>
+        <v>year2</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>2</v>
@@ -4455,7 +4484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>83</v>
       </c>
@@ -4469,7 +4498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>83</v>
       </c>
@@ -4483,7 +4512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
adding a missing VT file
</commit_message>
<xml_diff>
--- a/Syssettings.xlsx
+++ b/Syssettings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\adv demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\DemoS_ADV_Stuttgart061118\Adv_demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E136032-DC49-4707-8F1F-D9CA4D0A5B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4E1922-B091-4B17-9F4D-67A568C68FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -4197,7 +4197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4439,7 +4439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4454,13 +4456,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="137">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="str">
         <f>IF($A$1=1,"~TFM_MIG","~TFM_UPD")</f>
-        <v>~TFM_MIG</v>
+        <v>~TFM_UPD</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4475,7 +4477,7 @@
       </c>
       <c r="E4" s="5" t="str">
         <f>IF($A$1=1,"year2","year")</f>
-        <v>year2</v>
+        <v>year</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>2</v>

</xml_diff>